<commit_message>
Renamed tabs to include the prefix "le_"
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{743E413F-E4B5-44E4-9F29-C7CCEB08A233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECE7C5-51B8-4CB3-A0C8-77287EF885BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16632" yWindow="5556" windowWidth="12528" windowHeight="9420" tabRatio="712" activeTab="6" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="5" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inc" sheetId="15" r:id="rId1"/>
-    <sheet name="Hal" sheetId="18" r:id="rId2"/>
-    <sheet name="CFL" sheetId="16" r:id="rId3"/>
-    <sheet name="Fl" sheetId="17" r:id="rId4"/>
-    <sheet name="LED" sheetId="19" r:id="rId5"/>
-    <sheet name="HID" sheetId="20" r:id="rId6"/>
+    <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
+    <sheet name="le_Hal" sheetId="18" r:id="rId2"/>
+    <sheet name="le_CFL" sheetId="16" r:id="rId3"/>
+    <sheet name="le_Fl" sheetId="17" r:id="rId4"/>
+    <sheet name="le_LED" sheetId="19" r:id="rId5"/>
+    <sheet name="le_HID" sheetId="20" r:id="rId6"/>
     <sheet name="Figures" sheetId="21" r:id="rId7"/>
     <sheet name="Long-Run" sheetId="2" r:id="rId8"/>
     <sheet name="Short-Run" sheetId="7" r:id="rId9"/>
@@ -2049,7 +2049,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Inc!$A$2:$A$142</c:f>
+              <c:f>le_Inc!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -2481,7 +2481,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inc!$D$2:$D$142</c:f>
+              <c:f>le_Inc!$D$2:$D$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -2612,7 +2612,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hal!$A$2:$A$142</c:f>
+              <c:f>le_Hal!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3044,7 +3044,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hal!$D$2:$D$142</c:f>
+              <c:f>le_Hal!$D$2:$D$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3148,7 +3148,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>CFL!$A$2:$A$142</c:f>
+              <c:f>le_CFL!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3580,7 +3580,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CFL!$D$2:$D$142</c:f>
+              <c:f>le_CFL!$D$2:$D$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3672,7 +3672,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Fl!$A$2:$A$142</c:f>
+              <c:f>le_Fl!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -4104,7 +4104,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Fl!$D$2:$D$142</c:f>
+              <c:f>le_Fl!$D$2:$D$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -4190,7 +4190,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>LED!$A$2:$A$142</c:f>
+              <c:f>le_LED!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -4622,7 +4622,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>LED!$C$2:$C$142</c:f>
+              <c:f>le_LED!$C$2:$C$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -4702,7 +4702,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>HID!$A$2:$A$142</c:f>
+              <c:f>le_HID!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -5134,7 +5134,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>HID!$D$2:$D$142</c:f>
+              <c:f>le_HID!$D$2:$D$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -27826,7 +27826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0149D0B9-E1D4-4002-B3E6-86AD6A91C712}">
   <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -28575,7 +28575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7714C633-CAE6-4DA1-8F46-706D531B61FC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to caption for luminous efficacy graph. Added High Pressure Sodium Vapour lamp at 200W+ to lamps in figure
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7CF1AD-D6B6-4419-A723-35F05ACB4182}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65A3718-5C2F-4666-B508-B859C0D19E93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="5" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="5400" yWindow="0" windowWidth="12528" windowHeight="9420" tabRatio="712" activeTab="5" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
     <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="le_CFL" sheetId="16" r:id="rId3"/>
     <sheet name="le_Fl" sheetId="17" r:id="rId4"/>
     <sheet name="le_LED" sheetId="19" r:id="rId5"/>
-    <sheet name="le_HID" sheetId="20" r:id="rId6"/>
+    <sheet name="le_HPS200+" sheetId="20" r:id="rId6"/>
     <sheet name="Figures" sheetId="21" r:id="rId7"/>
     <sheet name="Long-Run" sheetId="2" r:id="rId8"/>
     <sheet name="Short-Run" sheetId="7" r:id="rId9"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="392">
   <si>
     <t>Tallow</t>
   </si>
@@ -1105,6 +1105,141 @@
   <si>
     <t>Technology</t>
   </si>
+  <si>
+    <t>GE Lucalox High Pressure Sodium Prototype</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20GE%20LU500.htm</t>
+  </si>
+  <si>
+    <t>Standard Lamps</t>
+  </si>
+  <si>
+    <t>GE Lucalox LU400/BD with External Amalgam Reservoir</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20GE%20LU400BD.htm</t>
+  </si>
+  <si>
+    <t>GE Lucalox LU250 Universal with Butterfly Crimp</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20GE%20LU250.htm</t>
+  </si>
+  <si>
+    <t>GE Lucalox LU1000 S52 with Voltage Fuse</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20GE%20LU1000.htm</t>
+  </si>
+  <si>
+    <t>Tesla SHC 400W Original HPS Design</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Tesla%20SHC400%20Nb-cup.htm</t>
+  </si>
+  <si>
+    <t>Stellox High Pressure Sodium</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Atlas%20SON250.htm</t>
+  </si>
+  <si>
+    <t>Tungsram TC400 2nd Generation</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Orion%20TC400.htm</t>
+  </si>
+  <si>
+    <t>Polamp WLS 400W 1st Generation</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Polamp%20WLS400.htm</t>
+  </si>
+  <si>
+    <t>Sylvania Lumalux LU200 HPS</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Sylvania%20LU200.htm</t>
+  </si>
+  <si>
+    <t>Tungsram LU250 with Double Wire Seals</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Tungsram%20LU250.htm</t>
+  </si>
+  <si>
+    <t>SON-T 1000W with Narrow Bore Nb Seals</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Thorn%20SONT1000.htm</t>
+  </si>
+  <si>
+    <t>High Pressure Sodium (&gt;200W)</t>
+  </si>
+  <si>
+    <t>Reflector Style</t>
+  </si>
+  <si>
+    <t>Osram Vialox NAV-R 310/360W</t>
+  </si>
+  <si>
+    <t>Reflux High Pressure Sodium with Reflector</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Reflux.htm</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Osram%20SONR310.htm</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Thorn%20SONTD1000.htm</t>
+  </si>
+  <si>
+    <t>Quartzray SON-TD 1000W-400V</t>
+  </si>
+  <si>
+    <t>Linear Style</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Osram%20SONL250.htm</t>
+  </si>
+  <si>
+    <t>Solarstream Linear Sodium SON-L 250W</t>
+  </si>
+  <si>
+    <t>Quartzray SON-TD 400W</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Thorn%20SONTD400.htm</t>
+  </si>
+  <si>
+    <t>Vialox Linear Sodium NAV-TS 400W</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Osram%20NAVTS400.htm</t>
+  </si>
+  <si>
+    <t>COBR Polam - WLS 400W Linear HP Sodium</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20COBR%20WLSTC400.htm</t>
+  </si>
+  <si>
+    <t>Philips Master GreenPower 1000W TD</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20Philips%20SONTD%20GreenPower%201000.htm</t>
+  </si>
+  <si>
+    <t>http://www.lamptech.co.uk/Spec%20Sheets/D%20SHP%20GE%20LU250-BD-S.htm</t>
+  </si>
+  <si>
+    <t>GE Lucalox LU250/BD/S with Superior Performance</t>
+  </si>
+  <si>
+    <t>Enhanced Efficacy Designs</t>
+  </si>
 </sst>
 </file>
 
@@ -4705,7 +4840,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>le_HID!$A$2:$A$142</c:f>
+              <c:f>'le_HPS200+'!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -5137,10 +5272,70 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>le_HID!$E$2:$E$142</c:f>
+              <c:f>'le_HPS200+'!$E$2:$E$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
+                <c:pt idx="85">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>117.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>137.5</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>139</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -29967,16 +30162,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0149D0B9-E1D4-4002-B3E6-86AD6A91C712}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -30010,7 +30207,7 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -30018,7 +30215,7 @@
         <v>1881</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -30026,7 +30223,7 @@
         <v>1882</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -30034,7 +30231,7 @@
         <v>1883</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -30042,7 +30239,7 @@
         <v>1884</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
       <c r="E6" s="120"/>
     </row>
@@ -30051,7 +30248,7 @@
         <v>1885</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -30059,7 +30256,7 @@
         <v>1886</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -30067,7 +30264,7 @@
         <v>1887</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -30075,7 +30272,7 @@
         <v>1888</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -30083,7 +30280,7 @@
         <v>1889</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -30091,7 +30288,7 @@
         <v>1890</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -30099,7 +30296,7 @@
         <v>1891</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -30107,7 +30304,7 @@
         <v>1892</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -30115,7 +30312,7 @@
         <v>1893</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -30123,7 +30320,7 @@
         <v>1894</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -30131,7 +30328,7 @@
         <v>1895</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -30139,7 +30336,7 @@
         <v>1896</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -30147,7 +30344,7 @@
         <v>1897</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -30155,7 +30352,7 @@
         <v>1898</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -30163,7 +30360,7 @@
         <v>1899</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -30171,7 +30368,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -30179,7 +30376,7 @@
         <v>1901</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -30187,7 +30384,7 @@
         <v>1902</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -30195,7 +30392,7 @@
         <v>1903</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -30203,7 +30400,7 @@
         <v>1904</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -30211,7 +30408,7 @@
         <v>1905</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -30219,7 +30416,7 @@
         <v>1906</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -30227,7 +30424,7 @@
         <v>1907</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -30235,7 +30432,7 @@
         <v>1908</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -30243,7 +30440,7 @@
         <v>1909</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -30251,7 +30448,7 @@
         <v>1910</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -30259,7 +30456,7 @@
         <v>1911</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -30267,7 +30464,7 @@
         <v>1912</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -30275,7 +30472,7 @@
         <v>1913</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -30283,7 +30480,7 @@
         <v>1914</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -30291,7 +30488,7 @@
         <v>1915</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -30299,7 +30496,7 @@
         <v>1916</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -30307,7 +30504,7 @@
         <v>1917</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -30315,7 +30512,7 @@
         <v>1918</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -30323,7 +30520,7 @@
         <v>1919</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -30331,7 +30528,7 @@
         <v>1920</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -30339,7 +30536,7 @@
         <v>1921</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -30347,7 +30544,7 @@
         <v>1922</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -30355,7 +30552,7 @@
         <v>1923</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -30363,7 +30560,7 @@
         <v>1924</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -30371,7 +30568,7 @@
         <v>1925</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -30379,7 +30576,7 @@
         <v>1926</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -30387,7 +30584,7 @@
         <v>1927</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -30395,7 +30592,7 @@
         <v>1928</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -30403,7 +30600,7 @@
         <v>1929</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -30411,7 +30608,7 @@
         <v>1930</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -30419,7 +30616,7 @@
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -30427,7 +30624,7 @@
         <v>1932</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -30435,7 +30632,7 @@
         <v>1933</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -30443,7 +30640,7 @@
         <v>1934</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -30451,7 +30648,7 @@
         <v>1935</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -30459,7 +30656,7 @@
         <v>1936</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -30467,7 +30664,7 @@
         <v>1937</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -30475,7 +30672,7 @@
         <v>1938</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -30483,7 +30680,7 @@
         <v>1939</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -30491,7 +30688,7 @@
         <v>1940</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -30499,7 +30696,7 @@
         <v>1941</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -30507,7 +30704,7 @@
         <v>1942</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -30515,7 +30712,7 @@
         <v>1943</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -30523,7 +30720,7 @@
         <v>1944</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -30531,7 +30728,7 @@
         <v>1945</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -30539,7 +30736,7 @@
         <v>1946</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -30547,7 +30744,7 @@
         <v>1947</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -30555,7 +30752,7 @@
         <v>1948</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -30563,7 +30760,7 @@
         <v>1949</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -30571,7 +30768,7 @@
         <v>1950</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -30579,7 +30776,7 @@
         <v>1951</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -30587,7 +30784,7 @@
         <v>1952</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -30595,7 +30792,7 @@
         <v>1953</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -30603,7 +30800,7 @@
         <v>1954</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -30611,7 +30808,7 @@
         <v>1955</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -30619,7 +30816,7 @@
         <v>1956</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -30627,7 +30824,7 @@
         <v>1957</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -30635,391 +30832,691 @@
         <v>1958</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>1959</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>1960</v>
       </c>
       <c r="B82" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>1961</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>1962</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>1963</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>1964</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>1965</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C87" t="s">
+        <v>349</v>
+      </c>
+      <c r="D87" t="s">
+        <v>347</v>
+      </c>
+      <c r="E87">
+        <v>100</v>
+      </c>
+      <c r="F87">
+        <v>500</v>
+      </c>
+      <c r="G87" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>1966</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>1967</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C89" t="s">
+        <v>349</v>
+      </c>
+      <c r="D89" t="s">
+        <v>356</v>
+      </c>
+      <c r="E89">
+        <v>110</v>
+      </c>
+      <c r="F89">
+        <v>400</v>
+      </c>
+      <c r="G89" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>1968</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>1969</v>
       </c>
       <c r="B91" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C91" t="s">
+        <v>349</v>
+      </c>
+      <c r="D91" t="s">
+        <v>358</v>
+      </c>
+      <c r="E91">
+        <v>100</v>
+      </c>
+      <c r="F91">
+        <v>250</v>
+      </c>
+      <c r="G91" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>1970</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>1971</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C93" t="s">
+        <v>349</v>
+      </c>
+      <c r="D93" t="s">
+        <v>350</v>
+      </c>
+      <c r="E93">
+        <v>117.5</v>
+      </c>
+      <c r="F93">
+        <v>400</v>
+      </c>
+      <c r="G93" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>1972</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>1973</v>
       </c>
       <c r="B95" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>1974</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>1975</v>
       </c>
       <c r="B97" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C97" t="s">
+        <v>349</v>
+      </c>
+      <c r="D97" t="s">
+        <v>360</v>
+      </c>
+      <c r="E97">
+        <v>110</v>
+      </c>
+      <c r="F97">
+        <v>400</v>
+      </c>
+      <c r="G97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>1976</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>1977</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C99" t="s">
+        <v>391</v>
+      </c>
+      <c r="D99" t="s">
+        <v>390</v>
+      </c>
+      <c r="E99">
+        <v>120</v>
+      </c>
+      <c r="F99">
+        <v>250</v>
+      </c>
+      <c r="G99" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>1978</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C100" t="s">
+        <v>349</v>
+      </c>
+      <c r="D100" t="s">
+        <v>362</v>
+      </c>
+      <c r="E100">
+        <v>110</v>
+      </c>
+      <c r="F100">
+        <v>400</v>
+      </c>
+      <c r="G100" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>1979</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>1980</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C102" t="s">
+        <v>349</v>
+      </c>
+      <c r="D102" t="s">
+        <v>354</v>
+      </c>
+      <c r="E102">
+        <v>140</v>
+      </c>
+      <c r="F102">
+        <v>1000</v>
+      </c>
+      <c r="G102" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>1981</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>1982</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C104" t="s">
+        <v>349</v>
+      </c>
+      <c r="D104" t="s">
+        <v>364</v>
+      </c>
+      <c r="E104">
+        <v>110</v>
+      </c>
+      <c r="F104">
+        <v>200</v>
+      </c>
+      <c r="G104" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>1983</v>
       </c>
       <c r="B105" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C105" t="s">
+        <v>349</v>
+      </c>
+      <c r="D105" t="s">
+        <v>352</v>
+      </c>
+      <c r="E105">
+        <v>110</v>
+      </c>
+      <c r="F105">
+        <v>250</v>
+      </c>
+      <c r="G105" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>1984</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>1985</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C107" t="s">
+        <v>349</v>
+      </c>
+      <c r="D107" t="s">
+        <v>366</v>
+      </c>
+      <c r="E107">
+        <v>108</v>
+      </c>
+      <c r="F107">
+        <v>250</v>
+      </c>
+      <c r="G107" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>1986</v>
       </c>
       <c r="B108" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>1987</v>
       </c>
       <c r="B109" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C109" t="s">
+        <v>378</v>
+      </c>
+      <c r="D109" t="s">
+        <v>381</v>
+      </c>
+      <c r="E109">
+        <v>120</v>
+      </c>
+      <c r="F109">
+        <v>400</v>
+      </c>
+      <c r="G109" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>1988</v>
       </c>
       <c r="B110" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C110" t="s">
+        <v>349</v>
+      </c>
+      <c r="D110" t="s">
+        <v>368</v>
+      </c>
+      <c r="E110">
+        <v>130</v>
+      </c>
+      <c r="F110">
+        <v>1000</v>
+      </c>
+      <c r="G110" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>1989</v>
       </c>
       <c r="B111" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C111" t="s">
+        <v>378</v>
+      </c>
+      <c r="D111" t="s">
+        <v>383</v>
+      </c>
+      <c r="E111">
+        <v>120</v>
+      </c>
+      <c r="F111">
+        <v>400</v>
+      </c>
+      <c r="G111" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>1990</v>
       </c>
       <c r="B112" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C112" t="s">
+        <v>378</v>
+      </c>
+      <c r="D112" t="s">
+        <v>377</v>
+      </c>
+      <c r="E112">
+        <v>137.5</v>
+      </c>
+      <c r="F112">
+        <v>1000</v>
+      </c>
+      <c r="G112" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>1991</v>
       </c>
       <c r="B113" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>1992</v>
       </c>
       <c r="B114" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C114" t="s">
+        <v>378</v>
+      </c>
+      <c r="D114" t="s">
+        <v>380</v>
+      </c>
+      <c r="E114">
+        <v>116</v>
+      </c>
+      <c r="F114">
+        <v>250</v>
+      </c>
+      <c r="G114" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>1993</v>
       </c>
       <c r="B115" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>1994</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117">
         <v>1995</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118">
         <v>1996</v>
       </c>
       <c r="B118" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119">
         <v>1997</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C119" t="s">
+        <v>378</v>
+      </c>
+      <c r="D119" t="s">
+        <v>385</v>
+      </c>
+      <c r="E119">
+        <v>110</v>
+      </c>
+      <c r="F119">
+        <v>400</v>
+      </c>
+      <c r="G119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120">
         <v>1998</v>
       </c>
       <c r="B120" t="s">
+        <v>370</v>
+      </c>
+      <c r="C120" t="s">
+        <v>371</v>
+      </c>
+      <c r="D120" t="s">
+        <v>372</v>
+      </c>
+      <c r="E120">
         <v>102</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="F120">
+        <v>360</v>
+      </c>
+      <c r="G120" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121">
         <v>1999</v>
       </c>
       <c r="B121" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122">
         <v>2000</v>
       </c>
       <c r="B122" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123">
         <v>2001</v>
       </c>
       <c r="B123" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124">
         <v>2002</v>
       </c>
       <c r="B124" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125">
         <v>2003</v>
       </c>
       <c r="B125" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C125" t="s">
+        <v>371</v>
+      </c>
+      <c r="D125" t="s">
+        <v>373</v>
+      </c>
+      <c r="E125">
+        <v>104</v>
+      </c>
+      <c r="F125">
+        <v>250</v>
+      </c>
+      <c r="G125" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126">
         <v>2004</v>
       </c>
       <c r="B126" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127">
         <v>2005</v>
       </c>
       <c r="B127" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>370</v>
+      </c>
+      <c r="C127" t="s">
+        <v>378</v>
+      </c>
+      <c r="D127" t="s">
+        <v>387</v>
+      </c>
+      <c r="E127">
+        <v>139</v>
+      </c>
+      <c r="F127">
+        <v>1000</v>
+      </c>
+      <c r="G127" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128">
         <v>2006</v>
       </c>
       <c r="B128" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -31027,7 +31524,7 @@
         <v>2007</v>
       </c>
       <c r="B129" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -31035,7 +31532,7 @@
         <v>2008</v>
       </c>
       <c r="B130" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -31043,7 +31540,7 @@
         <v>2009</v>
       </c>
       <c r="B131" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -31051,7 +31548,7 @@
         <v>2010</v>
       </c>
       <c r="B132" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -31059,7 +31556,7 @@
         <v>2011</v>
       </c>
       <c r="B133" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -31067,7 +31564,7 @@
         <v>2012</v>
       </c>
       <c r="B134" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -31075,7 +31572,7 @@
         <v>2013</v>
       </c>
       <c r="B135" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -31083,7 +31580,7 @@
         <v>2014</v>
       </c>
       <c r="B136" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -31091,7 +31588,7 @@
         <v>2015</v>
       </c>
       <c r="B137" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -31099,7 +31596,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -31107,7 +31604,7 @@
         <v>2017</v>
       </c>
       <c r="B139" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -31115,7 +31612,7 @@
         <v>2018</v>
       </c>
       <c r="B140" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -31123,7 +31620,7 @@
         <v>2019</v>
       </c>
       <c r="B141" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -31131,7 +31628,7 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
-        <v>102</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed legend. Added Type == LSPDD to identify lamps from the LSPDD when filtering for geom_label.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4736C5-867E-42E3-B503-5152DD525FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2494971-5E89-49EB-B091-E663617D852F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="5" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="3" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
     <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3768" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3770" uniqueCount="401">
   <si>
     <t>Tallow</t>
   </si>
@@ -1249,9 +1249,6 @@
     <t>Phillips Helios</t>
   </si>
   <si>
-    <t>Streetlight</t>
-  </si>
-  <si>
     <t>Globe Twister Energy Saver</t>
   </si>
   <si>
@@ -1268,6 +1265,9 @@
   </si>
   <si>
     <t>Phillips A19</t>
+  </si>
+  <si>
+    <t>LSPDD</t>
   </si>
 </sst>
 </file>
@@ -12167,7 +12167,7 @@
   <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView topLeftCell="A108" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13677,10 +13677,10 @@
         <v>42</v>
       </c>
       <c r="C135" t="s">
-        <v>272</v>
+        <v>400</v>
       </c>
       <c r="D135" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E135">
         <v>8.1</v>
@@ -13689,7 +13689,7 @@
         <v>40</v>
       </c>
       <c r="G135" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -24644,7 +24644,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
+      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -26047,7 +26047,7 @@
         <v>370</v>
       </c>
       <c r="C134" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="D134" t="s">
         <v>393</v>
@@ -26137,7 +26137,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G134" sqref="G134"/>
+      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27426,8 +27426,11 @@
       <c r="B134" t="s">
         <v>90</v>
       </c>
+      <c r="C134" t="s">
+        <v>400</v>
+      </c>
       <c r="D134" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E134">
         <v>61.1</v>
@@ -27436,7 +27439,7 @@
         <v>9</v>
       </c>
       <c r="G134" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -27548,9 +27551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB671D-7717-4C97-9193-8C24EFD9DC8A}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
+      <selection pane="bottomLeft" activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -28722,8 +28725,11 @@
       <c r="B136" t="s">
         <v>46</v>
       </c>
+      <c r="C136" t="s">
+        <v>400</v>
+      </c>
       <c r="D136" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E136">
         <v>75.5</v>
@@ -28732,7 +28738,7 @@
         <v>11</v>
       </c>
       <c r="G136" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -30335,7 +30341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0293270E-AF53-4651-A405-EC07D674C941}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added ifo to Lighting Efficacy data file.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2494971-5E89-49EB-B091-E663617D852F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1745D-C17E-45B3-B8D4-55F13DA11177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="3" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3770" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="401">
   <si>
     <t>Tallow</t>
   </si>
@@ -27553,7 +27553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E126" sqref="E126"/>
+      <selection pane="bottomLeft" activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -28335,6 +28335,9 @@
       <c r="B94" t="s">
         <v>46</v>
       </c>
+      <c r="C94" t="s">
+        <v>226</v>
+      </c>
       <c r="D94" t="s">
         <v>221</v>
       </c>
@@ -28355,6 +28358,9 @@
       <c r="B95" t="s">
         <v>46</v>
       </c>
+      <c r="C95" t="s">
+        <v>226</v>
+      </c>
       <c r="D95" t="s">
         <v>223</v>
       </c>
@@ -28591,6 +28597,9 @@
       <c r="B123" t="s">
         <v>46</v>
       </c>
+      <c r="C123" t="s">
+        <v>46</v>
+      </c>
       <c r="D123" t="s">
         <v>218</v>
       </c>
@@ -28664,6 +28673,9 @@
       <c r="B131" t="s">
         <v>46</v>
       </c>
+      <c r="C131" t="s">
+        <v>46</v>
+      </c>
       <c r="D131" t="s">
         <v>220</v>
       </c>
@@ -28684,6 +28696,9 @@
       <c r="B132" t="s">
         <v>46</v>
       </c>
+      <c r="C132" t="s">
+        <v>46</v>
+      </c>
       <c r="D132" t="s">
         <v>218</v>
       </c>
@@ -28748,6 +28763,9 @@
       <c r="B137" t="s">
         <v>46</v>
       </c>
+      <c r="C137" t="s">
+        <v>46</v>
+      </c>
       <c r="D137" t="s">
         <v>218</v>
       </c>
@@ -28765,6 +28783,9 @@
       <c r="B138" t="s">
         <v>46</v>
       </c>
+      <c r="C138" t="s">
+        <v>46</v>
+      </c>
       <c r="D138" t="s">
         <v>218</v>
       </c>
@@ -28785,6 +28806,9 @@
       <c r="B139" t="s">
         <v>46</v>
       </c>
+      <c r="C139" t="s">
+        <v>46</v>
+      </c>
       <c r="D139" t="s">
         <v>218</v>
       </c>
@@ -28805,6 +28829,9 @@
       <c r="B140" t="s">
         <v>46</v>
       </c>
+      <c r="C140" t="s">
+        <v>46</v>
+      </c>
       <c r="D140" t="s">
         <v>218</v>
       </c>
@@ -28825,6 +28852,9 @@
       <c r="B141" t="s">
         <v>46</v>
       </c>
+      <c r="C141" t="s">
+        <v>46</v>
+      </c>
       <c r="D141" t="s">
         <v>218</v>
       </c>
@@ -28843,6 +28873,9 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
+        <v>46</v>
+      </c>
+      <c r="C142" t="s">
         <v>46</v>
       </c>
       <c r="D142" t="s">

</xml_diff>

<commit_message>
Efficacy graph updated with selected lamps as a different shape and labels.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1745D-C17E-45B3-B8D4-55F13DA11177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF43BA5-A7CE-480C-8476-1D48C7CAA984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="3" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="401">
   <si>
     <t>Tallow</t>
   </si>
@@ -12166,7 +12166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9D9AE-BEA5-4CF9-A363-2955BA21CAB2}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
@@ -26135,9 +26135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892130B0-4D3E-4381-8355-A56FEEA0ADAB}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27272,6 +27272,9 @@
       <c r="B123" t="s">
         <v>90</v>
       </c>
+      <c r="C123" t="s">
+        <v>120</v>
+      </c>
       <c r="D123" t="s">
         <v>218</v>
       </c>
@@ -27485,6 +27488,9 @@
       <c r="B138" t="s">
         <v>90</v>
       </c>
+      <c r="C138" t="s">
+        <v>47</v>
+      </c>
       <c r="D138" t="s">
         <v>218</v>
       </c>
@@ -27504,6 +27510,9 @@
       </c>
       <c r="B139" t="s">
         <v>90</v>
+      </c>
+      <c r="C139" t="s">
+        <v>47</v>
       </c>
       <c r="D139" t="s">
         <v>218</v>
@@ -27552,7 +27561,7 @@
   <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed HAL to HPS in results and luminous effiacy graph - all works as expected.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4804A61A-D057-48CF-AB55-BA91F6F837F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA23385-954F-492E-AA3C-78527C4241B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11532" yWindow="2184" windowWidth="11508" windowHeight="9420" tabRatio="712" activeTab="3" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="11508" windowHeight="9420" tabRatio="712" activeTab="1" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
     <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
-    <sheet name="le_HPS&lt;100W" sheetId="22" r:id="rId2"/>
+    <sheet name="le_Hal" sheetId="18" r:id="rId2"/>
     <sheet name="le_CFL" sheetId="16" r:id="rId3"/>
     <sheet name="le_LED" sheetId="19" r:id="rId4"/>
-    <sheet name="Hal" sheetId="18" r:id="rId5"/>
+    <sheet name="HPS&lt;100W" sheetId="22" r:id="rId5"/>
     <sheet name="HPS200+" sheetId="20" r:id="rId6"/>
     <sheet name="Fl" sheetId="17" r:id="rId7"/>
     <sheet name="Figures" sheetId="21" r:id="rId8"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="431">
   <si>
     <t>Tallow</t>
   </si>
@@ -1353,6 +1353,12 @@
   </si>
   <si>
     <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2492</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2514</t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2873,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hal!$A$2:$A$142</c:f>
+              <c:f>le_Hal!$A$2:$A$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3299,7 +3305,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hal!$E$2:$E$142</c:f>
+              <c:f>le_Hal!$E$2:$E$142</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="141"/>
@@ -3359,6 +3365,9 @@
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>17.5</c:v>
@@ -31501,22 +31510,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B60507-60AE-40C8-BF7F-ED247905C63D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727D1E04-31A3-4998-85D9-AF32A9D150AF}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B142"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -31550,7 +31560,7 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -31558,7 +31568,7 @@
         <v>1881</v>
       </c>
       <c r="B3" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -31566,7 +31576,7 @@
         <v>1882</v>
       </c>
       <c r="B4" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -31574,7 +31584,7 @@
         <v>1883</v>
       </c>
       <c r="B5" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -31582,7 +31592,7 @@
         <v>1884</v>
       </c>
       <c r="B6" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="E6" s="120"/>
     </row>
@@ -31591,7 +31601,7 @@
         <v>1885</v>
       </c>
       <c r="B7" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -31599,7 +31609,7 @@
         <v>1886</v>
       </c>
       <c r="B8" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -31607,7 +31617,7 @@
         <v>1887</v>
       </c>
       <c r="B9" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -31615,7 +31625,7 @@
         <v>1888</v>
       </c>
       <c r="B10" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -31623,7 +31633,7 @@
         <v>1889</v>
       </c>
       <c r="B11" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -31631,7 +31641,7 @@
         <v>1890</v>
       </c>
       <c r="B12" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -31639,7 +31649,7 @@
         <v>1891</v>
       </c>
       <c r="B13" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -31647,7 +31657,7 @@
         <v>1892</v>
       </c>
       <c r="B14" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -31655,7 +31665,7 @@
         <v>1893</v>
       </c>
       <c r="B15" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -31663,7 +31673,7 @@
         <v>1894</v>
       </c>
       <c r="B16" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -31671,7 +31681,7 @@
         <v>1895</v>
       </c>
       <c r="B17" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -31679,7 +31689,7 @@
         <v>1896</v>
       </c>
       <c r="B18" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -31687,7 +31697,7 @@
         <v>1897</v>
       </c>
       <c r="B19" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -31695,7 +31705,7 @@
         <v>1898</v>
       </c>
       <c r="B20" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -31703,7 +31713,7 @@
         <v>1899</v>
       </c>
       <c r="B21" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -31711,7 +31721,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -31719,7 +31729,7 @@
         <v>1901</v>
       </c>
       <c r="B23" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -31727,7 +31737,7 @@
         <v>1902</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -31735,7 +31745,7 @@
         <v>1903</v>
       </c>
       <c r="B25" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -31743,7 +31753,7 @@
         <v>1904</v>
       </c>
       <c r="B26" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -31751,7 +31761,7 @@
         <v>1905</v>
       </c>
       <c r="B27" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -31759,7 +31769,7 @@
         <v>1906</v>
       </c>
       <c r="B28" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -31767,7 +31777,7 @@
         <v>1907</v>
       </c>
       <c r="B29" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -31775,7 +31785,7 @@
         <v>1908</v>
       </c>
       <c r="B30" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -31783,7 +31793,7 @@
         <v>1909</v>
       </c>
       <c r="B31" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -31791,7 +31801,7 @@
         <v>1910</v>
       </c>
       <c r="B32" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -31799,7 +31809,7 @@
         <v>1911</v>
       </c>
       <c r="B33" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -31807,7 +31817,7 @@
         <v>1912</v>
       </c>
       <c r="B34" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -31815,7 +31825,7 @@
         <v>1913</v>
       </c>
       <c r="B35" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -31823,7 +31833,7 @@
         <v>1914</v>
       </c>
       <c r="B36" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -31831,7 +31841,7 @@
         <v>1915</v>
       </c>
       <c r="B37" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -31839,7 +31849,7 @@
         <v>1916</v>
       </c>
       <c r="B38" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -31847,7 +31857,7 @@
         <v>1917</v>
       </c>
       <c r="B39" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -31855,7 +31865,7 @@
         <v>1918</v>
       </c>
       <c r="B40" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -31863,7 +31873,7 @@
         <v>1919</v>
       </c>
       <c r="B41" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -31871,7 +31881,7 @@
         <v>1920</v>
       </c>
       <c r="B42" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -31879,7 +31889,7 @@
         <v>1921</v>
       </c>
       <c r="B43" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -31887,7 +31897,7 @@
         <v>1922</v>
       </c>
       <c r="B44" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -31895,7 +31905,7 @@
         <v>1923</v>
       </c>
       <c r="B45" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -31903,7 +31913,7 @@
         <v>1924</v>
       </c>
       <c r="B46" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -31911,7 +31921,7 @@
         <v>1925</v>
       </c>
       <c r="B47" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -31919,7 +31929,7 @@
         <v>1926</v>
       </c>
       <c r="B48" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31927,7 +31937,7 @@
         <v>1927</v>
       </c>
       <c r="B49" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -31935,7 +31945,7 @@
         <v>1928</v>
       </c>
       <c r="B50" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -31943,7 +31953,7 @@
         <v>1929</v>
       </c>
       <c r="B51" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -31951,7 +31961,7 @@
         <v>1930</v>
       </c>
       <c r="B52" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -31959,7 +31969,7 @@
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -31967,7 +31977,7 @@
         <v>1932</v>
       </c>
       <c r="B54" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -31975,7 +31985,7 @@
         <v>1933</v>
       </c>
       <c r="B55" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -31983,7 +31993,7 @@
         <v>1934</v>
       </c>
       <c r="B56" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -31991,7 +32001,7 @@
         <v>1935</v>
       </c>
       <c r="B57" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -31999,7 +32009,7 @@
         <v>1936</v>
       </c>
       <c r="B58" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -32007,7 +32017,7 @@
         <v>1937</v>
       </c>
       <c r="B59" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -32015,7 +32025,7 @@
         <v>1938</v>
       </c>
       <c r="B60" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -32023,7 +32033,7 @@
         <v>1939</v>
       </c>
       <c r="B61" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -32031,7 +32041,7 @@
         <v>1940</v>
       </c>
       <c r="B62" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -32039,7 +32049,7 @@
         <v>1941</v>
       </c>
       <c r="B63" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -32047,7 +32057,7 @@
         <v>1942</v>
       </c>
       <c r="B64" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -32055,7 +32065,7 @@
         <v>1943</v>
       </c>
       <c r="B65" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -32063,7 +32073,7 @@
         <v>1944</v>
       </c>
       <c r="B66" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -32071,7 +32081,7 @@
         <v>1945</v>
       </c>
       <c r="B67" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -32079,7 +32089,7 @@
         <v>1946</v>
       </c>
       <c r="B68" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -32087,7 +32097,7 @@
         <v>1947</v>
       </c>
       <c r="B69" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -32095,7 +32105,7 @@
         <v>1948</v>
       </c>
       <c r="B70" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -32103,7 +32113,7 @@
         <v>1949</v>
       </c>
       <c r="B71" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -32111,7 +32121,7 @@
         <v>1950</v>
       </c>
       <c r="B72" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -32119,7 +32129,7 @@
         <v>1951</v>
       </c>
       <c r="B73" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -32127,7 +32137,7 @@
         <v>1952</v>
       </c>
       <c r="B74" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -32135,7 +32145,7 @@
         <v>1953</v>
       </c>
       <c r="B75" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -32143,7 +32153,7 @@
         <v>1954</v>
       </c>
       <c r="B76" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -32151,7 +32161,7 @@
         <v>1955</v>
       </c>
       <c r="B77" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -32159,7 +32169,7 @@
         <v>1956</v>
       </c>
       <c r="B78" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -32167,7 +32177,7 @@
         <v>1957</v>
       </c>
       <c r="B79" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -32175,7 +32185,7 @@
         <v>1958</v>
       </c>
       <c r="B80" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -32183,7 +32193,7 @@
         <v>1959</v>
       </c>
       <c r="B81" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -32191,7 +32201,7 @@
         <v>1960</v>
       </c>
       <c r="B82" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -32199,7 +32209,7 @@
         <v>1961</v>
       </c>
       <c r="B83" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -32207,7 +32217,7 @@
         <v>1962</v>
       </c>
       <c r="B84" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -32215,7 +32225,7 @@
         <v>1963</v>
       </c>
       <c r="B85" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -32223,7 +32233,22 @@
         <v>1964</v>
       </c>
       <c r="B86" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C86" t="s">
+        <v>278</v>
+      </c>
+      <c r="D86" t="s">
+        <v>279</v>
+      </c>
+      <c r="E86">
+        <v>21</v>
+      </c>
+      <c r="F86">
+        <v>500</v>
+      </c>
+      <c r="G86" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -32231,7 +32256,7 @@
         <v>1965</v>
       </c>
       <c r="B87" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -32239,7 +32264,22 @@
         <v>1966</v>
       </c>
       <c r="B88" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" t="s">
+        <v>283</v>
+      </c>
+      <c r="E88">
+        <v>26.2</v>
+      </c>
+      <c r="F88">
+        <v>420</v>
+      </c>
+      <c r="G88" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -32247,7 +32287,7 @@
         <v>1967</v>
       </c>
       <c r="B89" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -32255,7 +32295,7 @@
         <v>1968</v>
       </c>
       <c r="B90" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -32263,7 +32303,22 @@
         <v>1969</v>
       </c>
       <c r="B91" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C91" t="s">
+        <v>287</v>
+      </c>
+      <c r="D91" t="s">
+        <v>285</v>
+      </c>
+      <c r="E91">
+        <v>18</v>
+      </c>
+      <c r="F91">
+        <v>50</v>
+      </c>
+      <c r="G91" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -32271,22 +32326,7 @@
         <v>1970</v>
       </c>
       <c r="B92" t="s">
-        <v>423</v>
-      </c>
-      <c r="C92" t="s">
-        <v>349</v>
-      </c>
-      <c r="D92" t="s">
-        <v>393</v>
-      </c>
-      <c r="E92">
-        <v>80</v>
-      </c>
-      <c r="F92">
-        <v>125</v>
-      </c>
-      <c r="G92" t="s">
-        <v>394</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -32294,7 +32334,7 @@
         <v>1971</v>
       </c>
       <c r="B93" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -32302,7 +32342,7 @@
         <v>1972</v>
       </c>
       <c r="B94" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -32310,7 +32350,7 @@
         <v>1973</v>
       </c>
       <c r="B95" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -32318,7 +32358,7 @@
         <v>1974</v>
       </c>
       <c r="B96" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -32326,7 +32366,7 @@
         <v>1975</v>
       </c>
       <c r="B97" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -32334,22 +32374,7 @@
         <v>1976</v>
       </c>
       <c r="B98" t="s">
-        <v>423</v>
-      </c>
-      <c r="C98" t="s">
-        <v>349</v>
-      </c>
-      <c r="D98" t="s">
-        <v>395</v>
-      </c>
-      <c r="E98">
-        <v>82.9</v>
-      </c>
-      <c r="F98">
-        <v>70</v>
-      </c>
-      <c r="G98" t="s">
-        <v>396</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -32357,7 +32382,7 @@
         <v>1977</v>
       </c>
       <c r="B99" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -32365,7 +32390,7 @@
         <v>1978</v>
       </c>
       <c r="B100" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -32373,7 +32398,7 @@
         <v>1979</v>
       </c>
       <c r="B101" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -32381,22 +32406,7 @@
         <v>1980</v>
       </c>
       <c r="B102" t="s">
-        <v>423</v>
-      </c>
-      <c r="C102" t="s">
-        <v>349</v>
-      </c>
-      <c r="D102" t="s">
-        <v>397</v>
-      </c>
-      <c r="E102">
-        <v>66</v>
-      </c>
-      <c r="F102">
-        <v>50</v>
-      </c>
-      <c r="G102" s="120" t="s">
-        <v>399</v>
+        <v>43</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -32404,7 +32414,7 @@
         <v>1981</v>
       </c>
       <c r="B103" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -32412,22 +32422,7 @@
         <v>1982</v>
       </c>
       <c r="B104" t="s">
-        <v>423</v>
-      </c>
-      <c r="C104" t="s">
-        <v>370</v>
-      </c>
-      <c r="D104" t="s">
-        <v>414</v>
-      </c>
-      <c r="E104">
-        <v>57.1</v>
-      </c>
-      <c r="F104">
-        <v>70</v>
-      </c>
-      <c r="G104" t="s">
-        <v>415</v>
+        <v>43</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -32435,22 +32430,7 @@
         <v>1983</v>
       </c>
       <c r="B105" t="s">
-        <v>423</v>
-      </c>
-      <c r="C105" t="s">
-        <v>349</v>
-      </c>
-      <c r="D105" t="s">
-        <v>402</v>
-      </c>
-      <c r="E105">
-        <v>82.9</v>
-      </c>
-      <c r="F105">
-        <v>70</v>
-      </c>
-      <c r="G105" t="s">
-        <v>401</v>
+        <v>43</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -32458,7 +32438,7 @@
         <v>1984</v>
       </c>
       <c r="B106" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -32466,7 +32446,22 @@
         <v>1985</v>
       </c>
       <c r="B107" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C107" t="s">
+        <v>278</v>
+      </c>
+      <c r="D107" t="s">
+        <v>281</v>
+      </c>
+      <c r="E107">
+        <v>17</v>
+      </c>
+      <c r="F107">
+        <v>300</v>
+      </c>
+      <c r="G107" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -32474,7 +32469,22 @@
         <v>1986</v>
       </c>
       <c r="B108" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C108" t="s">
+        <v>291</v>
+      </c>
+      <c r="D108" t="s">
+        <v>294</v>
+      </c>
+      <c r="E108">
+        <v>16.8</v>
+      </c>
+      <c r="F108">
+        <v>250</v>
+      </c>
+      <c r="G108" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -32482,22 +32492,22 @@
         <v>1987</v>
       </c>
       <c r="B109" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C109" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="D109" t="s">
-        <v>404</v>
+        <v>324</v>
       </c>
       <c r="E109">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="F109">
         <v>50</v>
       </c>
-      <c r="G109" s="120" t="s">
-        <v>403</v>
+      <c r="G109" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -32505,7 +32515,22 @@
         <v>1988</v>
       </c>
       <c r="B110" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C110" t="s">
+        <v>323</v>
+      </c>
+      <c r="D110" t="s">
+        <v>328</v>
+      </c>
+      <c r="E110">
+        <v>18</v>
+      </c>
+      <c r="F110">
+        <v>50</v>
+      </c>
+      <c r="G110" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -32513,7 +32538,22 @@
         <v>1989</v>
       </c>
       <c r="B111" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C111" t="s">
+        <v>291</v>
+      </c>
+      <c r="D111" t="s">
+        <v>292</v>
+      </c>
+      <c r="E111">
+        <v>24</v>
+      </c>
+      <c r="F111">
+        <v>1000</v>
+      </c>
+      <c r="G111" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -32521,22 +32561,22 @@
         <v>1990</v>
       </c>
       <c r="B112" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C112" t="s">
-        <v>407</v>
+        <v>291</v>
       </c>
       <c r="D112" t="s">
-        <v>408</v>
+        <v>297</v>
       </c>
       <c r="E112">
-        <v>82.8</v>
+        <v>16.8</v>
       </c>
       <c r="F112">
-        <v>70</v>
+        <v>250</v>
       </c>
       <c r="G112" t="s">
-        <v>417</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -32544,22 +32584,22 @@
         <v>1991</v>
       </c>
       <c r="B113" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="D113" t="s">
-        <v>406</v>
+        <v>312</v>
       </c>
       <c r="E113">
-        <v>85.7</v>
+        <v>14.5</v>
       </c>
       <c r="F113">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G113" t="s">
-        <v>405</v>
+        <v>313</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -32567,22 +32607,22 @@
         <v>1992</v>
       </c>
       <c r="B114" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C114" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="D114" t="s">
-        <v>398</v>
+        <v>326</v>
       </c>
       <c r="E114">
-        <v>85.7</v>
+        <v>20</v>
       </c>
       <c r="F114">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="G114" t="s">
-        <v>400</v>
+        <v>327</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -32590,7 +32630,7 @@
         <v>1993</v>
       </c>
       <c r="B115" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -32598,7 +32638,22 @@
         <v>1994</v>
       </c>
       <c r="B116" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C116" t="s">
+        <v>311</v>
+      </c>
+      <c r="D116" t="s">
+        <v>314</v>
+      </c>
+      <c r="E116">
+        <v>14</v>
+      </c>
+      <c r="F116">
+        <v>60</v>
+      </c>
+      <c r="G116" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -32606,7 +32661,7 @@
         <v>1995</v>
       </c>
       <c r="B117" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -32614,22 +32669,7 @@
         <v>1996</v>
       </c>
       <c r="B118" t="s">
-        <v>423</v>
-      </c>
-      <c r="C118" t="s">
-        <v>390</v>
-      </c>
-      <c r="D118" t="s">
-        <v>412</v>
-      </c>
-      <c r="E118">
-        <v>100</v>
-      </c>
-      <c r="F118">
-        <v>100</v>
-      </c>
-      <c r="G118" t="s">
-        <v>411</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -32637,7 +32677,22 @@
         <v>1997</v>
       </c>
       <c r="B119" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C119" t="s">
+        <v>318</v>
+      </c>
+      <c r="D119" t="s">
+        <v>319</v>
+      </c>
+      <c r="E119">
+        <v>10.5</v>
+      </c>
+      <c r="F119">
+        <v>50</v>
+      </c>
+      <c r="G119" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -32645,7 +32700,7 @@
         <v>1998</v>
       </c>
       <c r="B120" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -32653,7 +32708,7 @@
         <v>1999</v>
       </c>
       <c r="B121" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -32661,7 +32716,7 @@
         <v>2000</v>
       </c>
       <c r="B122" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -32669,7 +32724,19 @@
         <v>2001</v>
       </c>
       <c r="B123" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C123" t="s">
+        <v>277</v>
+      </c>
+      <c r="D123" t="s">
+        <v>218</v>
+      </c>
+      <c r="E123">
+        <v>20</v>
+      </c>
+      <c r="G123" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -32677,7 +32744,7 @@
         <v>2002</v>
       </c>
       <c r="B124" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -32685,7 +32752,7 @@
         <v>2003</v>
       </c>
       <c r="B125" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -32693,7 +32760,22 @@
         <v>2004</v>
       </c>
       <c r="B126" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C126" t="s">
+        <v>311</v>
+      </c>
+      <c r="D126" t="s">
+        <v>316</v>
+      </c>
+      <c r="E126">
+        <v>13.7</v>
+      </c>
+      <c r="F126">
+        <v>60</v>
+      </c>
+      <c r="G126" s="120" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -32701,7 +32783,22 @@
         <v>2005</v>
       </c>
       <c r="B127" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C127" t="s">
+        <v>288</v>
+      </c>
+      <c r="D127" t="s">
+        <v>289</v>
+      </c>
+      <c r="E127">
+        <v>13.7</v>
+      </c>
+      <c r="F127">
+        <v>60</v>
+      </c>
+      <c r="G127" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -32709,7 +32806,22 @@
         <v>2006</v>
       </c>
       <c r="B128" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C128" t="s">
+        <v>318</v>
+      </c>
+      <c r="D128" t="s">
+        <v>321</v>
+      </c>
+      <c r="E128">
+        <v>12.3</v>
+      </c>
+      <c r="F128">
+        <v>40</v>
+      </c>
+      <c r="G128" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -32717,7 +32829,7 @@
         <v>2007</v>
       </c>
       <c r="B129" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -32725,22 +32837,22 @@
         <v>2008</v>
       </c>
       <c r="B130" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C130" t="s">
-        <v>390</v>
+        <v>298</v>
       </c>
       <c r="D130" t="s">
-        <v>413</v>
+        <v>299</v>
       </c>
       <c r="E130">
-        <v>94.3</v>
+        <v>20.7</v>
       </c>
       <c r="F130">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G130" t="s">
-        <v>416</v>
+        <v>300</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -32748,22 +32860,7 @@
         <v>2009</v>
       </c>
       <c r="B131" t="s">
-        <v>423</v>
-      </c>
-      <c r="C131" t="s">
-        <v>407</v>
-      </c>
-      <c r="D131" t="s">
-        <v>410</v>
-      </c>
-      <c r="E131">
-        <v>62.3</v>
-      </c>
-      <c r="F131">
-        <v>69</v>
-      </c>
-      <c r="G131" t="s">
-        <v>409</v>
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -32771,7 +32868,19 @@
         <v>2010</v>
       </c>
       <c r="B132" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C132" t="s">
+        <v>276</v>
+      </c>
+      <c r="D132" t="s">
+        <v>218</v>
+      </c>
+      <c r="E132">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="G132" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -32779,7 +32888,7 @@
         <v>2011</v>
       </c>
       <c r="B133" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -32787,22 +32896,22 @@
         <v>2012</v>
       </c>
       <c r="B134" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
       <c r="C134" t="s">
         <v>392</v>
       </c>
       <c r="D134" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="E134">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F134">
-        <v>100</v>
-      </c>
-      <c r="G134" t="s">
-        <v>391</v>
+        <v>65</v>
+      </c>
+      <c r="G134" s="120" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -32810,7 +32919,7 @@
         <v>2013</v>
       </c>
       <c r="B135" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -32818,7 +32927,7 @@
         <v>2014</v>
       </c>
       <c r="B136" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -32826,7 +32935,19 @@
         <v>2015</v>
       </c>
       <c r="B137" t="s">
-        <v>423</v>
+        <v>43</v>
+      </c>
+      <c r="C137" t="s">
+        <v>273</v>
+      </c>
+      <c r="D137" t="s">
+        <v>218</v>
+      </c>
+      <c r="E137">
+        <v>17.5</v>
+      </c>
+      <c r="G137" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -32834,7 +32955,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -32842,7 +32963,7 @@
         <v>2017</v>
       </c>
       <c r="B139" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -32850,7 +32971,7 @@
         <v>2018</v>
       </c>
       <c r="B140" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -32858,7 +32979,7 @@
         <v>2019</v>
       </c>
       <c r="B141" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -32866,13 +32987,13 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G102" r:id="rId1" xr:uid="{497818AE-E34B-47DC-9D02-3D4211664C35}"/>
-    <hyperlink ref="G109" r:id="rId2" xr:uid="{B2DFE39E-FBF9-4AEF-8AB5-BBACAF19AB80}"/>
+    <hyperlink ref="G126" r:id="rId1" xr:uid="{26AF3C9A-8692-410D-95F0-DE82A7A6CAB4}"/>
+    <hyperlink ref="G134" r:id="rId2" xr:uid="{306F7BBF-1505-4F63-8A27-5FA1563D0899}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34310,7 +34431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB671D-7717-4C97-9193-8C24EFD9DC8A}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F128" sqref="F128"/>
     </sheetView>
@@ -35659,23 +35780,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727D1E04-31A3-4998-85D9-AF32A9D150AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B60507-60AE-40C8-BF7F-ED247905C63D}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="29.44140625" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -35709,7 +35829,7 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -35717,7 +35837,7 @@
         <v>1881</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -35725,7 +35845,7 @@
         <v>1882</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -35733,7 +35853,7 @@
         <v>1883</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -35741,7 +35861,7 @@
         <v>1884</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="E6" s="120"/>
     </row>
@@ -35750,7 +35870,7 @@
         <v>1885</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -35758,7 +35878,7 @@
         <v>1886</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -35766,7 +35886,7 @@
         <v>1887</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -35774,7 +35894,7 @@
         <v>1888</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -35782,7 +35902,7 @@
         <v>1889</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -35790,7 +35910,7 @@
         <v>1890</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -35798,7 +35918,7 @@
         <v>1891</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -35806,7 +35926,7 @@
         <v>1892</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -35814,7 +35934,7 @@
         <v>1893</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -35822,7 +35942,7 @@
         <v>1894</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -35830,7 +35950,7 @@
         <v>1895</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -35838,7 +35958,7 @@
         <v>1896</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -35846,7 +35966,7 @@
         <v>1897</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -35854,7 +35974,7 @@
         <v>1898</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -35862,7 +35982,7 @@
         <v>1899</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -35870,7 +35990,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -35878,7 +35998,7 @@
         <v>1901</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -35886,7 +36006,7 @@
         <v>1902</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -35894,7 +36014,7 @@
         <v>1903</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -35902,7 +36022,7 @@
         <v>1904</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -35910,7 +36030,7 @@
         <v>1905</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -35918,7 +36038,7 @@
         <v>1906</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -35926,7 +36046,7 @@
         <v>1907</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -35934,7 +36054,7 @@
         <v>1908</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -35942,7 +36062,7 @@
         <v>1909</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -35950,7 +36070,7 @@
         <v>1910</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -35958,7 +36078,7 @@
         <v>1911</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -35966,7 +36086,7 @@
         <v>1912</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -35974,7 +36094,7 @@
         <v>1913</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -35982,7 +36102,7 @@
         <v>1914</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -35990,7 +36110,7 @@
         <v>1915</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -35998,7 +36118,7 @@
         <v>1916</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -36006,7 +36126,7 @@
         <v>1917</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -36014,7 +36134,7 @@
         <v>1918</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -36022,7 +36142,7 @@
         <v>1919</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -36030,7 +36150,7 @@
         <v>1920</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -36038,7 +36158,7 @@
         <v>1921</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -36046,7 +36166,7 @@
         <v>1922</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -36054,7 +36174,7 @@
         <v>1923</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -36062,7 +36182,7 @@
         <v>1924</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -36070,7 +36190,7 @@
         <v>1925</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -36078,7 +36198,7 @@
         <v>1926</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -36086,7 +36206,7 @@
         <v>1927</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -36094,7 +36214,7 @@
         <v>1928</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -36102,7 +36222,7 @@
         <v>1929</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -36110,7 +36230,7 @@
         <v>1930</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -36118,7 +36238,7 @@
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -36126,7 +36246,7 @@
         <v>1932</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -36134,7 +36254,7 @@
         <v>1933</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -36142,7 +36262,7 @@
         <v>1934</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -36150,7 +36270,7 @@
         <v>1935</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -36158,7 +36278,7 @@
         <v>1936</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -36166,7 +36286,7 @@
         <v>1937</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -36174,7 +36294,7 @@
         <v>1938</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -36182,7 +36302,7 @@
         <v>1939</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -36190,7 +36310,7 @@
         <v>1940</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -36198,7 +36318,7 @@
         <v>1941</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -36206,7 +36326,7 @@
         <v>1942</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -36214,7 +36334,7 @@
         <v>1943</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -36222,7 +36342,7 @@
         <v>1944</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -36230,7 +36350,7 @@
         <v>1945</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -36238,7 +36358,7 @@
         <v>1946</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -36246,7 +36366,7 @@
         <v>1947</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -36254,7 +36374,7 @@
         <v>1948</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -36262,7 +36382,7 @@
         <v>1949</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -36270,7 +36390,7 @@
         <v>1950</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -36278,7 +36398,7 @@
         <v>1951</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -36286,7 +36406,7 @@
         <v>1952</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -36294,7 +36414,7 @@
         <v>1953</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -36302,7 +36422,7 @@
         <v>1954</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -36310,7 +36430,7 @@
         <v>1955</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -36318,7 +36438,7 @@
         <v>1956</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -36326,7 +36446,7 @@
         <v>1957</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -36334,7 +36454,7 @@
         <v>1958</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -36342,7 +36462,7 @@
         <v>1959</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -36350,7 +36470,7 @@
         <v>1960</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -36358,7 +36478,7 @@
         <v>1961</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -36366,7 +36486,7 @@
         <v>1962</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -36374,7 +36494,7 @@
         <v>1963</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -36382,22 +36502,7 @@
         <v>1964</v>
       </c>
       <c r="B86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C86" t="s">
-        <v>278</v>
-      </c>
-      <c r="D86" t="s">
-        <v>279</v>
-      </c>
-      <c r="E86">
-        <v>21</v>
-      </c>
-      <c r="F86">
-        <v>500</v>
-      </c>
-      <c r="G86" t="s">
-        <v>280</v>
+        <v>423</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -36405,7 +36510,7 @@
         <v>1965</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -36413,22 +36518,7 @@
         <v>1966</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
-      </c>
-      <c r="C88" t="s">
-        <v>278</v>
-      </c>
-      <c r="D88" t="s">
-        <v>283</v>
-      </c>
-      <c r="E88">
-        <v>26.2</v>
-      </c>
-      <c r="F88">
-        <v>420</v>
-      </c>
-      <c r="G88" t="s">
-        <v>284</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -36436,7 +36526,7 @@
         <v>1967</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -36444,7 +36534,7 @@
         <v>1968</v>
       </c>
       <c r="B90" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -36452,22 +36542,7 @@
         <v>1969</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
-      </c>
-      <c r="C91" t="s">
-        <v>287</v>
-      </c>
-      <c r="D91" t="s">
-        <v>285</v>
-      </c>
-      <c r="E91">
-        <v>18</v>
-      </c>
-      <c r="F91">
-        <v>50</v>
-      </c>
-      <c r="G91" t="s">
-        <v>286</v>
+        <v>423</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -36475,7 +36550,22 @@
         <v>1970</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C92" t="s">
+        <v>349</v>
+      </c>
+      <c r="D92" t="s">
+        <v>393</v>
+      </c>
+      <c r="E92">
+        <v>80</v>
+      </c>
+      <c r="F92">
+        <v>125</v>
+      </c>
+      <c r="G92" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -36483,7 +36573,7 @@
         <v>1971</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -36491,7 +36581,7 @@
         <v>1972</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -36499,7 +36589,7 @@
         <v>1973</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -36507,7 +36597,7 @@
         <v>1974</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -36515,7 +36605,7 @@
         <v>1975</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -36523,7 +36613,22 @@
         <v>1976</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D98" t="s">
+        <v>395</v>
+      </c>
+      <c r="E98">
+        <v>82.9</v>
+      </c>
+      <c r="F98">
+        <v>70</v>
+      </c>
+      <c r="G98" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -36531,7 +36636,7 @@
         <v>1977</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -36539,7 +36644,7 @@
         <v>1978</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -36547,7 +36652,7 @@
         <v>1979</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -36555,7 +36660,22 @@
         <v>1980</v>
       </c>
       <c r="B102" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C102" t="s">
+        <v>349</v>
+      </c>
+      <c r="D102" t="s">
+        <v>397</v>
+      </c>
+      <c r="E102">
+        <v>66</v>
+      </c>
+      <c r="F102">
+        <v>50</v>
+      </c>
+      <c r="G102" s="120" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -36563,7 +36683,7 @@
         <v>1981</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -36571,7 +36691,22 @@
         <v>1982</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C104" t="s">
+        <v>370</v>
+      </c>
+      <c r="D104" t="s">
+        <v>414</v>
+      </c>
+      <c r="E104">
+        <v>57.1</v>
+      </c>
+      <c r="F104">
+        <v>70</v>
+      </c>
+      <c r="G104" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -36579,7 +36714,22 @@
         <v>1983</v>
       </c>
       <c r="B105" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C105" t="s">
+        <v>349</v>
+      </c>
+      <c r="D105" t="s">
+        <v>402</v>
+      </c>
+      <c r="E105">
+        <v>82.9</v>
+      </c>
+      <c r="F105">
+        <v>70</v>
+      </c>
+      <c r="G105" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -36587,7 +36737,7 @@
         <v>1984</v>
       </c>
       <c r="B106" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -36595,22 +36745,7 @@
         <v>1985</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
-      </c>
-      <c r="C107" t="s">
-        <v>278</v>
-      </c>
-      <c r="D107" t="s">
-        <v>281</v>
-      </c>
-      <c r="E107">
-        <v>17</v>
-      </c>
-      <c r="F107">
-        <v>300</v>
-      </c>
-      <c r="G107" t="s">
-        <v>282</v>
+        <v>423</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -36618,22 +36753,7 @@
         <v>1986</v>
       </c>
       <c r="B108" t="s">
-        <v>43</v>
-      </c>
-      <c r="C108" t="s">
-        <v>291</v>
-      </c>
-      <c r="D108" t="s">
-        <v>294</v>
-      </c>
-      <c r="E108">
-        <v>16.8</v>
-      </c>
-      <c r="F108">
-        <v>250</v>
-      </c>
-      <c r="G108" t="s">
-        <v>295</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -36641,22 +36761,22 @@
         <v>1987</v>
       </c>
       <c r="B109" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="C109" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="D109" t="s">
-        <v>324</v>
+        <v>404</v>
       </c>
       <c r="E109">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="F109">
         <v>50</v>
       </c>
-      <c r="G109" t="s">
-        <v>325</v>
+      <c r="G109" s="120" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -36664,22 +36784,7 @@
         <v>1988</v>
       </c>
       <c r="B110" t="s">
-        <v>43</v>
-      </c>
-      <c r="C110" t="s">
-        <v>323</v>
-      </c>
-      <c r="D110" t="s">
-        <v>328</v>
-      </c>
-      <c r="E110">
-        <v>18</v>
-      </c>
-      <c r="F110">
-        <v>50</v>
-      </c>
-      <c r="G110" t="s">
-        <v>329</v>
+        <v>423</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -36687,22 +36792,7 @@
         <v>1989</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
-      </c>
-      <c r="C111" t="s">
-        <v>291</v>
-      </c>
-      <c r="D111" t="s">
-        <v>292</v>
-      </c>
-      <c r="E111">
-        <v>24</v>
-      </c>
-      <c r="F111">
-        <v>1000</v>
-      </c>
-      <c r="G111" t="s">
-        <v>293</v>
+        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -36710,22 +36800,22 @@
         <v>1990</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="C112" t="s">
-        <v>291</v>
+        <v>407</v>
       </c>
       <c r="D112" t="s">
-        <v>297</v>
+        <v>408</v>
       </c>
       <c r="E112">
-        <v>16.8</v>
+        <v>82.8</v>
       </c>
       <c r="F112">
-        <v>250</v>
+        <v>70</v>
       </c>
       <c r="G112" t="s">
-        <v>296</v>
+        <v>417</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -36733,22 +36823,22 @@
         <v>1991</v>
       </c>
       <c r="B113" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="C113" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="D113" t="s">
-        <v>312</v>
+        <v>406</v>
       </c>
       <c r="E113">
-        <v>14.5</v>
+        <v>85.7</v>
       </c>
       <c r="F113">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G113" t="s">
-        <v>313</v>
+        <v>405</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -36756,22 +36846,22 @@
         <v>1992</v>
       </c>
       <c r="B114" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="C114" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="D114" t="s">
-        <v>326</v>
+        <v>398</v>
       </c>
       <c r="E114">
-        <v>20</v>
+        <v>85.7</v>
       </c>
       <c r="F114">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G114" t="s">
-        <v>327</v>
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -36779,7 +36869,7 @@
         <v>1993</v>
       </c>
       <c r="B115" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -36787,22 +36877,7 @@
         <v>1994</v>
       </c>
       <c r="B116" t="s">
-        <v>43</v>
-      </c>
-      <c r="C116" t="s">
-        <v>311</v>
-      </c>
-      <c r="D116" t="s">
-        <v>314</v>
-      </c>
-      <c r="E116">
-        <v>14</v>
-      </c>
-      <c r="F116">
-        <v>60</v>
-      </c>
-      <c r="G116" t="s">
-        <v>315</v>
+        <v>423</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -36810,7 +36885,7 @@
         <v>1995</v>
       </c>
       <c r="B117" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -36818,7 +36893,22 @@
         <v>1996</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C118" t="s">
+        <v>390</v>
+      </c>
+      <c r="D118" t="s">
+        <v>412</v>
+      </c>
+      <c r="E118">
+        <v>100</v>
+      </c>
+      <c r="F118">
+        <v>100</v>
+      </c>
+      <c r="G118" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -36826,22 +36916,7 @@
         <v>1997</v>
       </c>
       <c r="B119" t="s">
-        <v>43</v>
-      </c>
-      <c r="C119" t="s">
-        <v>318</v>
-      </c>
-      <c r="D119" t="s">
-        <v>319</v>
-      </c>
-      <c r="E119">
-        <v>10.5</v>
-      </c>
-      <c r="F119">
-        <v>50</v>
-      </c>
-      <c r="G119" t="s">
-        <v>320</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -36849,7 +36924,7 @@
         <v>1998</v>
       </c>
       <c r="B120" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -36857,7 +36932,7 @@
         <v>1999</v>
       </c>
       <c r="B121" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -36865,7 +36940,7 @@
         <v>2000</v>
       </c>
       <c r="B122" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -36873,19 +36948,7 @@
         <v>2001</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
-      </c>
-      <c r="C123" t="s">
-        <v>277</v>
-      </c>
-      <c r="D123" t="s">
-        <v>218</v>
-      </c>
-      <c r="E123">
-        <v>20</v>
-      </c>
-      <c r="G123" t="s">
-        <v>153</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -36893,7 +36956,7 @@
         <v>2002</v>
       </c>
       <c r="B124" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -36901,7 +36964,7 @@
         <v>2003</v>
       </c>
       <c r="B125" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -36909,22 +36972,7 @@
         <v>2004</v>
       </c>
       <c r="B126" t="s">
-        <v>43</v>
-      </c>
-      <c r="C126" t="s">
-        <v>311</v>
-      </c>
-      <c r="D126" t="s">
-        <v>316</v>
-      </c>
-      <c r="E126">
-        <v>13.7</v>
-      </c>
-      <c r="F126">
-        <v>60</v>
-      </c>
-      <c r="G126" s="120" t="s">
-        <v>317</v>
+        <v>423</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -36932,22 +36980,7 @@
         <v>2005</v>
       </c>
       <c r="B127" t="s">
-        <v>43</v>
-      </c>
-      <c r="C127" t="s">
-        <v>288</v>
-      </c>
-      <c r="D127" t="s">
-        <v>289</v>
-      </c>
-      <c r="E127">
-        <v>13.7</v>
-      </c>
-      <c r="F127">
-        <v>60</v>
-      </c>
-      <c r="G127" t="s">
-        <v>290</v>
+        <v>423</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -36955,22 +36988,7 @@
         <v>2006</v>
       </c>
       <c r="B128" t="s">
-        <v>43</v>
-      </c>
-      <c r="C128" t="s">
-        <v>318</v>
-      </c>
-      <c r="D128" t="s">
-        <v>321</v>
-      </c>
-      <c r="E128">
-        <v>12.3</v>
-      </c>
-      <c r="F128">
-        <v>40</v>
-      </c>
-      <c r="G128" t="s">
-        <v>322</v>
+        <v>423</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -36978,7 +36996,7 @@
         <v>2007</v>
       </c>
       <c r="B129" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -36986,22 +37004,22 @@
         <v>2008</v>
       </c>
       <c r="B130" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="C130" t="s">
-        <v>298</v>
+        <v>390</v>
       </c>
       <c r="D130" t="s">
-        <v>299</v>
+        <v>413</v>
       </c>
       <c r="E130">
-        <v>20.7</v>
+        <v>94.3</v>
       </c>
       <c r="F130">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G130" t="s">
-        <v>300</v>
+        <v>416</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -37009,7 +37027,22 @@
         <v>2009</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C131" t="s">
+        <v>407</v>
+      </c>
+      <c r="D131" t="s">
+        <v>410</v>
+      </c>
+      <c r="E131">
+        <v>62.3</v>
+      </c>
+      <c r="F131">
+        <v>69</v>
+      </c>
+      <c r="G131" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -37017,19 +37050,7 @@
         <v>2010</v>
       </c>
       <c r="B132" t="s">
-        <v>43</v>
-      </c>
-      <c r="C132" t="s">
-        <v>276</v>
-      </c>
-      <c r="D132" t="s">
-        <v>218</v>
-      </c>
-      <c r="E132">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="G132" t="s">
-        <v>227</v>
+        <v>423</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -37037,7 +37058,7 @@
         <v>2011</v>
       </c>
       <c r="B133" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -37045,7 +37066,22 @@
         <v>2012</v>
       </c>
       <c r="B134" t="s">
-        <v>43</v>
+        <v>423</v>
+      </c>
+      <c r="C134" t="s">
+        <v>392</v>
+      </c>
+      <c r="D134" t="s">
+        <v>420</v>
+      </c>
+      <c r="E134">
+        <v>85</v>
+      </c>
+      <c r="F134">
+        <v>100</v>
+      </c>
+      <c r="G134" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -37053,7 +37089,7 @@
         <v>2013</v>
       </c>
       <c r="B135" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -37061,7 +37097,7 @@
         <v>2014</v>
       </c>
       <c r="B136" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -37069,19 +37105,7 @@
         <v>2015</v>
       </c>
       <c r="B137" t="s">
-        <v>43</v>
-      </c>
-      <c r="C137" t="s">
-        <v>273</v>
-      </c>
-      <c r="D137" t="s">
-        <v>218</v>
-      </c>
-      <c r="E137">
-        <v>17.5</v>
-      </c>
-      <c r="G137" t="s">
-        <v>228</v>
+        <v>423</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -37089,7 +37113,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -37097,7 +37121,7 @@
         <v>2017</v>
       </c>
       <c r="B139" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -37105,7 +37129,7 @@
         <v>2018</v>
       </c>
       <c r="B140" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -37113,7 +37137,7 @@
         <v>2019</v>
       </c>
       <c r="B141" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -37121,12 +37145,13 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
-        <v>43</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G126" r:id="rId1" xr:uid="{26AF3C9A-8692-410D-95F0-DE82A7A6CAB4}"/>
+    <hyperlink ref="G102" r:id="rId1" xr:uid="{497818AE-E34B-47DC-9D02-3D4211664C35}"/>
+    <hyperlink ref="G109" r:id="rId2" xr:uid="{B2DFE39E-FBF9-4AEF-8AB5-BBACAF19AB80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Halogen -> Halogen (HAL) in luminous efficacy graph.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA23385-954F-492E-AA3C-78527C4241B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA36FFC-56D7-4058-88BF-775A4F84F3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="11508" windowHeight="9420" tabRatio="712" activeTab="1" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="1" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
     <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="432">
   <si>
     <t>Tallow</t>
   </si>
@@ -1359,6 +1359,9 @@
   </si>
   <si>
     <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2514</t>
+  </si>
+  <si>
+    <t>Halogen (HAL)</t>
   </si>
 </sst>
 </file>
@@ -31513,14 +31516,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727D1E04-31A3-4998-85D9-AF32A9D150AF}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G135" sqref="G135"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
     <col min="5" max="5" width="29.44140625" customWidth="1"/>
@@ -31560,7 +31563,7 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -31568,7 +31571,7 @@
         <v>1881</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -31576,7 +31579,7 @@
         <v>1882</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -31584,7 +31587,7 @@
         <v>1883</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -31592,7 +31595,7 @@
         <v>1884</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="E6" s="120"/>
     </row>
@@ -31601,7 +31604,7 @@
         <v>1885</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -31609,7 +31612,7 @@
         <v>1886</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -31617,7 +31620,7 @@
         <v>1887</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -31625,7 +31628,7 @@
         <v>1888</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -31633,7 +31636,7 @@
         <v>1889</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -31641,7 +31644,7 @@
         <v>1890</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -31649,7 +31652,7 @@
         <v>1891</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -31657,7 +31660,7 @@
         <v>1892</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -31665,7 +31668,7 @@
         <v>1893</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -31673,7 +31676,7 @@
         <v>1894</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -31681,7 +31684,7 @@
         <v>1895</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -31689,7 +31692,7 @@
         <v>1896</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -31697,7 +31700,7 @@
         <v>1897</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -31705,7 +31708,7 @@
         <v>1898</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -31713,7 +31716,7 @@
         <v>1899</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -31721,7 +31724,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -31729,7 +31732,7 @@
         <v>1901</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -31737,7 +31740,7 @@
         <v>1902</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -31745,7 +31748,7 @@
         <v>1903</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -31753,7 +31756,7 @@
         <v>1904</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -31761,7 +31764,7 @@
         <v>1905</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -31769,7 +31772,7 @@
         <v>1906</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -31777,7 +31780,7 @@
         <v>1907</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -31785,7 +31788,7 @@
         <v>1908</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -31793,7 +31796,7 @@
         <v>1909</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -31801,7 +31804,7 @@
         <v>1910</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -31809,7 +31812,7 @@
         <v>1911</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -31817,7 +31820,7 @@
         <v>1912</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -31825,7 +31828,7 @@
         <v>1913</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -31833,7 +31836,7 @@
         <v>1914</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -31841,7 +31844,7 @@
         <v>1915</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -31849,7 +31852,7 @@
         <v>1916</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -31857,7 +31860,7 @@
         <v>1917</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -31865,7 +31868,7 @@
         <v>1918</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -31873,7 +31876,7 @@
         <v>1919</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -31881,7 +31884,7 @@
         <v>1920</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -31889,7 +31892,7 @@
         <v>1921</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -31897,7 +31900,7 @@
         <v>1922</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -31905,7 +31908,7 @@
         <v>1923</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -31913,7 +31916,7 @@
         <v>1924</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -31921,7 +31924,7 @@
         <v>1925</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -31929,7 +31932,7 @@
         <v>1926</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31937,7 +31940,7 @@
         <v>1927</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -31945,7 +31948,7 @@
         <v>1928</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -31953,7 +31956,7 @@
         <v>1929</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -31961,7 +31964,7 @@
         <v>1930</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -31969,7 +31972,7 @@
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -31977,7 +31980,7 @@
         <v>1932</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -31985,7 +31988,7 @@
         <v>1933</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -31993,7 +31996,7 @@
         <v>1934</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -32001,7 +32004,7 @@
         <v>1935</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -32009,7 +32012,7 @@
         <v>1936</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -32017,7 +32020,7 @@
         <v>1937</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -32025,7 +32028,7 @@
         <v>1938</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -32033,7 +32036,7 @@
         <v>1939</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -32041,7 +32044,7 @@
         <v>1940</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -32049,7 +32052,7 @@
         <v>1941</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -32057,7 +32060,7 @@
         <v>1942</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -32065,7 +32068,7 @@
         <v>1943</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -32073,7 +32076,7 @@
         <v>1944</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -32081,7 +32084,7 @@
         <v>1945</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -32089,7 +32092,7 @@
         <v>1946</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -32097,7 +32100,7 @@
         <v>1947</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -32105,7 +32108,7 @@
         <v>1948</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -32113,7 +32116,7 @@
         <v>1949</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -32121,7 +32124,7 @@
         <v>1950</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -32129,7 +32132,7 @@
         <v>1951</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -32137,7 +32140,7 @@
         <v>1952</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -32145,7 +32148,7 @@
         <v>1953</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -32153,7 +32156,7 @@
         <v>1954</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -32161,7 +32164,7 @@
         <v>1955</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -32169,7 +32172,7 @@
         <v>1956</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -32177,7 +32180,7 @@
         <v>1957</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -32185,7 +32188,7 @@
         <v>1958</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -32193,7 +32196,7 @@
         <v>1959</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -32201,7 +32204,7 @@
         <v>1960</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -32209,7 +32212,7 @@
         <v>1961</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -32217,7 +32220,7 @@
         <v>1962</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -32225,7 +32228,7 @@
         <v>1963</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -32233,7 +32236,7 @@
         <v>1964</v>
       </c>
       <c r="B86" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C86" t="s">
         <v>278</v>
@@ -32256,7 +32259,7 @@
         <v>1965</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -32264,7 +32267,7 @@
         <v>1966</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C88" t="s">
         <v>278</v>
@@ -32287,7 +32290,7 @@
         <v>1967</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -32295,7 +32298,7 @@
         <v>1968</v>
       </c>
       <c r="B90" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -32303,7 +32306,7 @@
         <v>1969</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C91" t="s">
         <v>287</v>
@@ -32326,7 +32329,7 @@
         <v>1970</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -32334,7 +32337,7 @@
         <v>1971</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -32342,7 +32345,7 @@
         <v>1972</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -32350,7 +32353,7 @@
         <v>1973</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -32358,7 +32361,7 @@
         <v>1974</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -32366,7 +32369,7 @@
         <v>1975</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -32374,7 +32377,7 @@
         <v>1976</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -32382,7 +32385,7 @@
         <v>1977</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -32390,7 +32393,7 @@
         <v>1978</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -32398,7 +32401,7 @@
         <v>1979</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -32406,7 +32409,7 @@
         <v>1980</v>
       </c>
       <c r="B102" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -32414,7 +32417,7 @@
         <v>1981</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -32422,7 +32425,7 @@
         <v>1982</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -32430,7 +32433,7 @@
         <v>1983</v>
       </c>
       <c r="B105" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -32438,7 +32441,7 @@
         <v>1984</v>
       </c>
       <c r="B106" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -32446,7 +32449,7 @@
         <v>1985</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C107" t="s">
         <v>278</v>
@@ -32469,7 +32472,7 @@
         <v>1986</v>
       </c>
       <c r="B108" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C108" t="s">
         <v>291</v>
@@ -32492,7 +32495,7 @@
         <v>1987</v>
       </c>
       <c r="B109" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C109" t="s">
         <v>323</v>
@@ -32515,7 +32518,7 @@
         <v>1988</v>
       </c>
       <c r="B110" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C110" t="s">
         <v>323</v>
@@ -32538,7 +32541,7 @@
         <v>1989</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C111" t="s">
         <v>291</v>
@@ -32561,7 +32564,7 @@
         <v>1990</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C112" t="s">
         <v>291</v>
@@ -32584,7 +32587,7 @@
         <v>1991</v>
       </c>
       <c r="B113" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C113" t="s">
         <v>311</v>
@@ -32607,7 +32610,7 @@
         <v>1992</v>
       </c>
       <c r="B114" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C114" t="s">
         <v>323</v>
@@ -32630,7 +32633,7 @@
         <v>1993</v>
       </c>
       <c r="B115" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -32638,7 +32641,7 @@
         <v>1994</v>
       </c>
       <c r="B116" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C116" t="s">
         <v>311</v>
@@ -32661,7 +32664,7 @@
         <v>1995</v>
       </c>
       <c r="B117" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -32669,7 +32672,7 @@
         <v>1996</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -32677,7 +32680,7 @@
         <v>1997</v>
       </c>
       <c r="B119" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C119" t="s">
         <v>318</v>
@@ -32700,7 +32703,7 @@
         <v>1998</v>
       </c>
       <c r="B120" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -32708,7 +32711,7 @@
         <v>1999</v>
       </c>
       <c r="B121" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -32716,7 +32719,7 @@
         <v>2000</v>
       </c>
       <c r="B122" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -32724,7 +32727,7 @@
         <v>2001</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C123" t="s">
         <v>277</v>
@@ -32744,7 +32747,7 @@
         <v>2002</v>
       </c>
       <c r="B124" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -32752,7 +32755,7 @@
         <v>2003</v>
       </c>
       <c r="B125" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -32760,7 +32763,7 @@
         <v>2004</v>
       </c>
       <c r="B126" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C126" t="s">
         <v>311</v>
@@ -32783,7 +32786,7 @@
         <v>2005</v>
       </c>
       <c r="B127" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C127" t="s">
         <v>288</v>
@@ -32806,7 +32809,7 @@
         <v>2006</v>
       </c>
       <c r="B128" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C128" t="s">
         <v>318</v>
@@ -32829,7 +32832,7 @@
         <v>2007</v>
       </c>
       <c r="B129" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -32837,7 +32840,7 @@
         <v>2008</v>
       </c>
       <c r="B130" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
@@ -32860,7 +32863,7 @@
         <v>2009</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -32868,7 +32871,7 @@
         <v>2010</v>
       </c>
       <c r="B132" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C132" t="s">
         <v>276</v>
@@ -32888,7 +32891,7 @@
         <v>2011</v>
       </c>
       <c r="B133" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -32896,7 +32899,7 @@
         <v>2012</v>
       </c>
       <c r="B134" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C134" t="s">
         <v>392</v>
@@ -32919,7 +32922,7 @@
         <v>2013</v>
       </c>
       <c r="B135" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -32927,7 +32930,7 @@
         <v>2014</v>
       </c>
       <c r="B136" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -32935,7 +32938,7 @@
         <v>2015</v>
       </c>
       <c r="B137" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
       <c r="C137" t="s">
         <v>273</v>
@@ -32955,7 +32958,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -32963,7 +32966,7 @@
         <v>2017</v>
       </c>
       <c r="B139" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -32971,7 +32974,7 @@
         <v>2018</v>
       </c>
       <c r="B140" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -32979,7 +32982,7 @@
         <v>2019</v>
       </c>
       <c r="B141" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -32987,7 +32990,7 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
-        <v>43</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added INC lamp between 700-100lm. Changed lamp_list and lamp in luminous efficacy graph.
</commit_message>
<xml_diff>
--- a/Data/Lighting_Efficacy_Data.xlsx
+++ b/Data/Lighting_Efficacy_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA36FFC-56D7-4058-88BF-775A4F84F3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFCE287-683D-42C1-9B8D-BC8B5BE676F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" activeTab="1" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="712" xr2:uid="{846965A8-6FAB-48E0-BA8A-E1207C0888FB}"/>
   </bookViews>
   <sheets>
     <sheet name="le_Inc" sheetId="15" r:id="rId1"/>
@@ -1346,9 +1346,6 @@
     <t>Light-emitting diode (LED)</t>
   </si>
   <si>
-    <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2557</t>
-  </si>
-  <si>
     <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2538</t>
   </si>
   <si>
@@ -1362,6 +1359,9 @@
   </si>
   <si>
     <t>Halogen (HAL)</t>
+  </si>
+  <si>
+    <t>http://galileo.graphycs.cegepsherbrooke.qc.ca/app/en/lamps/2552</t>
   </si>
 </sst>
 </file>
@@ -2831,7 +2831,7 @@
                   <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>17.600000000000001</c:v>
+                  <c:v>14.1</c:v>
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>10.3</c:v>
@@ -12263,8 +12263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9D9AE-BEA5-4CF9-A363-2955BA21CAB2}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13780,13 +13780,13 @@
         <v>419</v>
       </c>
       <c r="E135">
-        <v>17.600000000000001</v>
+        <v>14.1</v>
       </c>
       <c r="F135">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="G135" s="120" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -13868,7 +13868,6 @@
     <hyperlink ref="G112" r:id="rId7" xr:uid="{4E67B11E-2CAD-4D19-BCCE-959A0E4359B8}"/>
     <hyperlink ref="G57" r:id="rId8" xr:uid="{55B98824-5519-41A0-96BA-BD12BCACFAE5}"/>
     <hyperlink ref="G47" r:id="rId9" xr:uid="{C4C7DE45-5EA8-4FDB-A560-444F5C59CD9B}"/>
-    <hyperlink ref="G135" r:id="rId10" xr:uid="{6B978241-D7F8-4FFC-A991-6E2D75773435}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31516,9 +31515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727D1E04-31A3-4998-85D9-AF32A9D150AF}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B142"/>
+      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31563,7 +31562,7 @@
         <v>1880</v>
       </c>
       <c r="B2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -31571,7 +31570,7 @@
         <v>1881</v>
       </c>
       <c r="B3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -31579,7 +31578,7 @@
         <v>1882</v>
       </c>
       <c r="B4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -31587,7 +31586,7 @@
         <v>1883</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -31595,7 +31594,7 @@
         <v>1884</v>
       </c>
       <c r="B6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E6" s="120"/>
     </row>
@@ -31604,7 +31603,7 @@
         <v>1885</v>
       </c>
       <c r="B7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -31612,7 +31611,7 @@
         <v>1886</v>
       </c>
       <c r="B8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -31620,7 +31619,7 @@
         <v>1887</v>
       </c>
       <c r="B9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -31628,7 +31627,7 @@
         <v>1888</v>
       </c>
       <c r="B10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -31636,7 +31635,7 @@
         <v>1889</v>
       </c>
       <c r="B11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -31644,7 +31643,7 @@
         <v>1890</v>
       </c>
       <c r="B12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -31652,7 +31651,7 @@
         <v>1891</v>
       </c>
       <c r="B13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -31660,7 +31659,7 @@
         <v>1892</v>
       </c>
       <c r="B14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -31668,7 +31667,7 @@
         <v>1893</v>
       </c>
       <c r="B15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -31676,7 +31675,7 @@
         <v>1894</v>
       </c>
       <c r="B16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -31684,7 +31683,7 @@
         <v>1895</v>
       </c>
       <c r="B17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -31692,7 +31691,7 @@
         <v>1896</v>
       </c>
       <c r="B18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -31700,7 +31699,7 @@
         <v>1897</v>
       </c>
       <c r="B19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -31708,7 +31707,7 @@
         <v>1898</v>
       </c>
       <c r="B20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -31716,7 +31715,7 @@
         <v>1899</v>
       </c>
       <c r="B21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -31724,7 +31723,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -31732,7 +31731,7 @@
         <v>1901</v>
       </c>
       <c r="B23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -31740,7 +31739,7 @@
         <v>1902</v>
       </c>
       <c r="B24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -31748,7 +31747,7 @@
         <v>1903</v>
       </c>
       <c r="B25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -31756,7 +31755,7 @@
         <v>1904</v>
       </c>
       <c r="B26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -31764,7 +31763,7 @@
         <v>1905</v>
       </c>
       <c r="B27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -31772,7 +31771,7 @@
         <v>1906</v>
       </c>
       <c r="B28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -31780,7 +31779,7 @@
         <v>1907</v>
       </c>
       <c r="B29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -31788,7 +31787,7 @@
         <v>1908</v>
       </c>
       <c r="B30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -31796,7 +31795,7 @@
         <v>1909</v>
       </c>
       <c r="B31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -31804,7 +31803,7 @@
         <v>1910</v>
       </c>
       <c r="B32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -31812,7 +31811,7 @@
         <v>1911</v>
       </c>
       <c r="B33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -31820,7 +31819,7 @@
         <v>1912</v>
       </c>
       <c r="B34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -31828,7 +31827,7 @@
         <v>1913</v>
       </c>
       <c r="B35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -31836,7 +31835,7 @@
         <v>1914</v>
       </c>
       <c r="B36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -31844,7 +31843,7 @@
         <v>1915</v>
       </c>
       <c r="B37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -31852,7 +31851,7 @@
         <v>1916</v>
       </c>
       <c r="B38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -31860,7 +31859,7 @@
         <v>1917</v>
       </c>
       <c r="B39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -31868,7 +31867,7 @@
         <v>1918</v>
       </c>
       <c r="B40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -31876,7 +31875,7 @@
         <v>1919</v>
       </c>
       <c r="B41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -31884,7 +31883,7 @@
         <v>1920</v>
       </c>
       <c r="B42" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -31892,7 +31891,7 @@
         <v>1921</v>
       </c>
       <c r="B43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -31900,7 +31899,7 @@
         <v>1922</v>
       </c>
       <c r="B44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -31908,7 +31907,7 @@
         <v>1923</v>
       </c>
       <c r="B45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -31916,7 +31915,7 @@
         <v>1924</v>
       </c>
       <c r="B46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -31924,7 +31923,7 @@
         <v>1925</v>
       </c>
       <c r="B47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -31932,7 +31931,7 @@
         <v>1926</v>
       </c>
       <c r="B48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31940,7 +31939,7 @@
         <v>1927</v>
       </c>
       <c r="B49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -31948,7 +31947,7 @@
         <v>1928</v>
       </c>
       <c r="B50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -31956,7 +31955,7 @@
         <v>1929</v>
       </c>
       <c r="B51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -31964,7 +31963,7 @@
         <v>1930</v>
       </c>
       <c r="B52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -31972,7 +31971,7 @@
         <v>1931</v>
       </c>
       <c r="B53" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -31980,7 +31979,7 @@
         <v>1932</v>
       </c>
       <c r="B54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -31988,7 +31987,7 @@
         <v>1933</v>
       </c>
       <c r="B55" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -31996,7 +31995,7 @@
         <v>1934</v>
       </c>
       <c r="B56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -32004,7 +32003,7 @@
         <v>1935</v>
       </c>
       <c r="B57" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -32012,7 +32011,7 @@
         <v>1936</v>
       </c>
       <c r="B58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -32020,7 +32019,7 @@
         <v>1937</v>
       </c>
       <c r="B59" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -32028,7 +32027,7 @@
         <v>1938</v>
       </c>
       <c r="B60" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -32036,7 +32035,7 @@
         <v>1939</v>
       </c>
       <c r="B61" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -32044,7 +32043,7 @@
         <v>1940</v>
       </c>
       <c r="B62" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -32052,7 +32051,7 @@
         <v>1941</v>
       </c>
       <c r="B63" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -32060,7 +32059,7 @@
         <v>1942</v>
       </c>
       <c r="B64" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -32068,7 +32067,7 @@
         <v>1943</v>
       </c>
       <c r="B65" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -32076,7 +32075,7 @@
         <v>1944</v>
       </c>
       <c r="B66" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -32084,7 +32083,7 @@
         <v>1945</v>
       </c>
       <c r="B67" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -32092,7 +32091,7 @@
         <v>1946</v>
       </c>
       <c r="B68" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -32100,7 +32099,7 @@
         <v>1947</v>
       </c>
       <c r="B69" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -32108,7 +32107,7 @@
         <v>1948</v>
       </c>
       <c r="B70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -32116,7 +32115,7 @@
         <v>1949</v>
       </c>
       <c r="B71" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -32124,7 +32123,7 @@
         <v>1950</v>
       </c>
       <c r="B72" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -32132,7 +32131,7 @@
         <v>1951</v>
       </c>
       <c r="B73" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -32140,7 +32139,7 @@
         <v>1952</v>
       </c>
       <c r="B74" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -32148,7 +32147,7 @@
         <v>1953</v>
       </c>
       <c r="B75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -32156,7 +32155,7 @@
         <v>1954</v>
       </c>
       <c r="B76" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -32164,7 +32163,7 @@
         <v>1955</v>
       </c>
       <c r="B77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -32172,7 +32171,7 @@
         <v>1956</v>
       </c>
       <c r="B78" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -32180,7 +32179,7 @@
         <v>1957</v>
       </c>
       <c r="B79" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -32188,7 +32187,7 @@
         <v>1958</v>
       </c>
       <c r="B80" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -32196,7 +32195,7 @@
         <v>1959</v>
       </c>
       <c r="B81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -32204,7 +32203,7 @@
         <v>1960</v>
       </c>
       <c r="B82" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -32212,7 +32211,7 @@
         <v>1961</v>
       </c>
       <c r="B83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -32220,7 +32219,7 @@
         <v>1962</v>
       </c>
       <c r="B84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -32228,7 +32227,7 @@
         <v>1963</v>
       </c>
       <c r="B85" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -32236,7 +32235,7 @@
         <v>1964</v>
       </c>
       <c r="B86" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C86" t="s">
         <v>278</v>
@@ -32259,7 +32258,7 @@
         <v>1965</v>
       </c>
       <c r="B87" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -32267,7 +32266,7 @@
         <v>1966</v>
       </c>
       <c r="B88" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C88" t="s">
         <v>278</v>
@@ -32290,7 +32289,7 @@
         <v>1967</v>
       </c>
       <c r="B89" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -32298,7 +32297,7 @@
         <v>1968</v>
       </c>
       <c r="B90" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -32306,7 +32305,7 @@
         <v>1969</v>
       </c>
       <c r="B91" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C91" t="s">
         <v>287</v>
@@ -32329,7 +32328,7 @@
         <v>1970</v>
       </c>
       <c r="B92" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -32337,7 +32336,7 @@
         <v>1971</v>
       </c>
       <c r="B93" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -32345,7 +32344,7 @@
         <v>1972</v>
       </c>
       <c r="B94" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -32353,7 +32352,7 @@
         <v>1973</v>
       </c>
       <c r="B95" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -32361,7 +32360,7 @@
         <v>1974</v>
       </c>
       <c r="B96" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -32369,7 +32368,7 @@
         <v>1975</v>
       </c>
       <c r="B97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -32377,7 +32376,7 @@
         <v>1976</v>
       </c>
       <c r="B98" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -32385,7 +32384,7 @@
         <v>1977</v>
       </c>
       <c r="B99" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -32393,7 +32392,7 @@
         <v>1978</v>
       </c>
       <c r="B100" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -32401,7 +32400,7 @@
         <v>1979</v>
       </c>
       <c r="B101" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -32409,7 +32408,7 @@
         <v>1980</v>
       </c>
       <c r="B102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -32417,7 +32416,7 @@
         <v>1981</v>
       </c>
       <c r="B103" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -32425,7 +32424,7 @@
         <v>1982</v>
       </c>
       <c r="B104" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -32433,7 +32432,7 @@
         <v>1983</v>
       </c>
       <c r="B105" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -32441,7 +32440,7 @@
         <v>1984</v>
       </c>
       <c r="B106" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -32449,7 +32448,7 @@
         <v>1985</v>
       </c>
       <c r="B107" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C107" t="s">
         <v>278</v>
@@ -32472,7 +32471,7 @@
         <v>1986</v>
       </c>
       <c r="B108" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C108" t="s">
         <v>291</v>
@@ -32495,7 +32494,7 @@
         <v>1987</v>
       </c>
       <c r="B109" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C109" t="s">
         <v>323</v>
@@ -32518,7 +32517,7 @@
         <v>1988</v>
       </c>
       <c r="B110" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C110" t="s">
         <v>323</v>
@@ -32541,7 +32540,7 @@
         <v>1989</v>
       </c>
       <c r="B111" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C111" t="s">
         <v>291</v>
@@ -32564,7 +32563,7 @@
         <v>1990</v>
       </c>
       <c r="B112" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C112" t="s">
         <v>291</v>
@@ -32587,7 +32586,7 @@
         <v>1991</v>
       </c>
       <c r="B113" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C113" t="s">
         <v>311</v>
@@ -32610,7 +32609,7 @@
         <v>1992</v>
       </c>
       <c r="B114" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C114" t="s">
         <v>323</v>
@@ -32633,7 +32632,7 @@
         <v>1993</v>
       </c>
       <c r="B115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -32641,7 +32640,7 @@
         <v>1994</v>
       </c>
       <c r="B116" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C116" t="s">
         <v>311</v>
@@ -32664,7 +32663,7 @@
         <v>1995</v>
       </c>
       <c r="B117" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -32672,7 +32671,7 @@
         <v>1996</v>
       </c>
       <c r="B118" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -32680,7 +32679,7 @@
         <v>1997</v>
       </c>
       <c r="B119" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C119" t="s">
         <v>318</v>
@@ -32703,7 +32702,7 @@
         <v>1998</v>
       </c>
       <c r="B120" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -32711,7 +32710,7 @@
         <v>1999</v>
       </c>
       <c r="B121" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -32719,7 +32718,7 @@
         <v>2000</v>
       </c>
       <c r="B122" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -32727,7 +32726,7 @@
         <v>2001</v>
       </c>
       <c r="B123" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C123" t="s">
         <v>277</v>
@@ -32747,7 +32746,7 @@
         <v>2002</v>
       </c>
       <c r="B124" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -32755,7 +32754,7 @@
         <v>2003</v>
       </c>
       <c r="B125" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -32763,7 +32762,7 @@
         <v>2004</v>
       </c>
       <c r="B126" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C126" t="s">
         <v>311</v>
@@ -32786,7 +32785,7 @@
         <v>2005</v>
       </c>
       <c r="B127" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C127" t="s">
         <v>288</v>
@@ -32809,7 +32808,7 @@
         <v>2006</v>
       </c>
       <c r="B128" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C128" t="s">
         <v>318</v>
@@ -32832,7 +32831,7 @@
         <v>2007</v>
       </c>
       <c r="B129" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -32840,7 +32839,7 @@
         <v>2008</v>
       </c>
       <c r="B130" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C130" t="s">
         <v>298</v>
@@ -32863,7 +32862,7 @@
         <v>2009</v>
       </c>
       <c r="B131" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -32871,7 +32870,7 @@
         <v>2010</v>
       </c>
       <c r="B132" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C132" t="s">
         <v>276</v>
@@ -32891,7 +32890,7 @@
         <v>2011</v>
       </c>
       <c r="B133" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -32899,13 +32898,13 @@
         <v>2012</v>
       </c>
       <c r="B134" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C134" t="s">
         <v>392</v>
       </c>
       <c r="D134" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E134">
         <v>11</v>
@@ -32914,7 +32913,7 @@
         <v>65</v>
       </c>
       <c r="G134" s="120" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -32922,7 +32921,7 @@
         <v>2013</v>
       </c>
       <c r="B135" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -32930,7 +32929,7 @@
         <v>2014</v>
       </c>
       <c r="B136" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -32938,7 +32937,7 @@
         <v>2015</v>
       </c>
       <c r="B137" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C137" t="s">
         <v>273</v>
@@ -32958,7 +32957,7 @@
         <v>2016</v>
       </c>
       <c r="B138" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -32966,7 +32965,7 @@
         <v>2017</v>
       </c>
       <c r="B139" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -32974,7 +32973,7 @@
         <v>2018</v>
       </c>
       <c r="B140" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -32982,7 +32981,7 @@
         <v>2019</v>
       </c>
       <c r="B141" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -32990,7 +32989,7 @@
         <v>2020</v>
       </c>
       <c r="B142" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -34329,7 +34328,7 @@
         <v>15</v>
       </c>
       <c r="G136" s="120" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -35628,7 +35627,7 @@
         <v>10</v>
       </c>
       <c r="G135" s="120" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="136" spans="1:7">

</xml_diff>